<commit_message>
map is plotting with pipe info
still uncropped, but otherwise looking good.
</commit_message>
<xml_diff>
--- a/data/kimberlite_coords.xlsx
+++ b/data/kimberlite_coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerzeigler/Documents/Flowers Lab/Arctic Kimberlite/canda-ahe-kimberlite-map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AF3EB5-B867-4740-834C-C9D06B36B42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D7B71D-FB09-354D-8ECB-022AF91BBB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="3460" windowWidth="27640" windowHeight="16440" xr2:uid="{271A1990-3C0E-BB45-A5DB-FD6F620B4979}"/>
+    <workbookView xWindow="920" yWindow="3460" windowWidth="21460" windowHeight="16520" xr2:uid="{271A1990-3C0E-BB45-A5DB-FD6F620B4979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="96">
   <si>
     <t>pipe</t>
   </si>
@@ -46,19 +46,328 @@
   </si>
   <si>
     <t>Thrift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">method </t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>processed?</t>
+  </si>
+  <si>
+    <t>picked?</t>
+  </si>
+  <si>
+    <t>transect</t>
+  </si>
+  <si>
+    <t>Thrift01</t>
+  </si>
+  <si>
+    <t>Thrift02</t>
+  </si>
+  <si>
+    <t>Thrift04</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>coronation gulf</t>
+  </si>
+  <si>
+    <t>Thrift-2</t>
+  </si>
+  <si>
+    <t>Thift KIA09</t>
+  </si>
+  <si>
+    <t>Thirft03</t>
+  </si>
+  <si>
+    <t>Thrift-A</t>
+  </si>
+  <si>
+    <t>Hydra-1</t>
+  </si>
+  <si>
+    <t>Hydra01</t>
+  </si>
+  <si>
+    <t>Hydra-KIA09</t>
+  </si>
+  <si>
+    <t>Hydra02</t>
+  </si>
+  <si>
+    <t>Hydra-flow banded</t>
+  </si>
+  <si>
+    <t>Hydra03</t>
+  </si>
+  <si>
+    <t>Kikerk-1</t>
+  </si>
+  <si>
+    <t>Kikerk01</t>
+  </si>
+  <si>
+    <t>Kikerk KIA09</t>
+  </si>
+  <si>
+    <t>Kikerk02</t>
+  </si>
+  <si>
+    <t>Perseus KIA09</t>
+  </si>
+  <si>
+    <t>Perseus01</t>
+  </si>
+  <si>
+    <t>Artemisia ART-2</t>
+  </si>
+  <si>
+    <t>Artemisia01</t>
+  </si>
+  <si>
+    <t>Jericho</t>
+  </si>
+  <si>
+    <t>Jericho01</t>
+  </si>
+  <si>
+    <t>Victoria Island- MGS</t>
+  </si>
+  <si>
+    <t>Victoria01</t>
+  </si>
+  <si>
+    <t>original_name</t>
+  </si>
+  <si>
+    <t>Transect1</t>
+  </si>
+  <si>
+    <t>Hydra</t>
+  </si>
+  <si>
+    <t>keep?</t>
+  </si>
+  <si>
+    <t>Kikerk</t>
+  </si>
+  <si>
+    <t>Perseus</t>
+  </si>
+  <si>
+    <t>Artemisia</t>
+  </si>
+  <si>
+    <t>King Eider</t>
+  </si>
+  <si>
+    <t>victoria island</t>
+  </si>
+  <si>
+    <t xml:space="preserve">somerset island </t>
+  </si>
+  <si>
+    <t>Batty Bay Blow 12</t>
+  </si>
+  <si>
+    <t>Jos</t>
+  </si>
+  <si>
+    <t>Ham</t>
+  </si>
+  <si>
+    <t>Elwin Bay</t>
+  </si>
+  <si>
+    <t>Cresswell Bay</t>
+  </si>
+  <si>
+    <t>Peuyuk, phase C</t>
+  </si>
+  <si>
+    <t>age_Ma</t>
+  </si>
+  <si>
+    <t>P2O5_wt%</t>
+  </si>
+  <si>
+    <t>Batty01</t>
+  </si>
+  <si>
+    <t>Jos01</t>
+  </si>
+  <si>
+    <t>Ham01</t>
+  </si>
+  <si>
+    <t>Elwin01</t>
+  </si>
+  <si>
+    <t>Cresswell01</t>
+  </si>
+  <si>
+    <t>Peuyuk01</t>
+  </si>
+  <si>
+    <t>PHA 90-K12 B</t>
+  </si>
+  <si>
+    <t>PHA 90-J1A</t>
+  </si>
+  <si>
+    <t>LH 86-53</t>
+  </si>
+  <si>
+    <t>PHA 90-E4A</t>
+  </si>
+  <si>
+    <t>KIA 92-CB</t>
+  </si>
+  <si>
+    <t>PHA 90-PC1</t>
+  </si>
+  <si>
+    <t>0.3 - 0.6 (2)</t>
+  </si>
+  <si>
+    <t>uncertainty_Ma</t>
+  </si>
+  <si>
+    <t>1.09 -1.28 (2)</t>
+  </si>
+  <si>
+    <t>U-Pb pvk</t>
+  </si>
+  <si>
+    <t>0.4 - 0.77 (2)</t>
+  </si>
+  <si>
+    <t>0.19 (3)</t>
+  </si>
+  <si>
+    <t>0.24 - 0.90 (7)</t>
+  </si>
+  <si>
+    <t>Rb-Sr phlogopite Composite</t>
+  </si>
+  <si>
+    <t>lac de gras</t>
+  </si>
+  <si>
+    <t>Eddie</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>C13</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>slave</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>these 'slave' samples are the ones bruce is doing mantle xenocryst studies on</t>
+  </si>
+  <si>
+    <t>Anuri</t>
+  </si>
+  <si>
+    <t>Ranch Lake</t>
+  </si>
+  <si>
+    <t>DryBones Bay</t>
+  </si>
+  <si>
+    <t>Tli Kwi Cho</t>
+  </si>
+  <si>
+    <t>Gahcho Kue</t>
+  </si>
+  <si>
+    <t>Snap Lake</t>
+  </si>
+  <si>
+    <t>U-Pb zircon</t>
+  </si>
+  <si>
+    <t>0.42 (2)</t>
+  </si>
+  <si>
+    <t>Rb-Sr phlogopite</t>
+  </si>
+  <si>
+    <t>0.56 (1)</t>
+  </si>
+  <si>
+    <t>0.52 - 0.71 (4)</t>
+  </si>
+  <si>
+    <t>0.33 - 0.40 (3)</t>
+  </si>
+  <si>
+    <t>Rb-Sr phlogopite (revised)</t>
+  </si>
+  <si>
+    <t>Fox</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,8 +390,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,37 +715,1150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DF6E0F1-3EB2-664F-BBCF-15D4BA25F41E}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
         <v>67.170439999999999</v>
       </c>
-      <c r="C2">
+      <c r="F2">
         <v>-113.04048</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2">
+        <v>534.20000000000005</v>
+      </c>
+      <c r="I2">
+        <v>2.8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" t="b">
+        <v>1</v>
+      </c>
+      <c r="L2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>67.170439999999999</v>
+      </c>
+      <c r="F3">
+        <v>-113.04048</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3">
+        <v>534.20000000000005</v>
+      </c>
+      <c r="I3">
+        <v>2.8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>69</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <v>67.170439999999999</v>
+      </c>
+      <c r="F4">
+        <v>-113.04048</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4">
+        <v>534.20000000000005</v>
+      </c>
+      <c r="I4">
+        <v>2.8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>67.170439999999999</v>
+      </c>
+      <c r="F5">
+        <v>-113.04048</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5">
+        <v>534.20000000000005</v>
+      </c>
+      <c r="I5">
+        <v>2.8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
+      <c r="L5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6">
+        <v>67.140267005300004</v>
+      </c>
+      <c r="F6">
+        <v>-113.216152206</v>
+      </c>
+      <c r="H6">
+        <v>601.6</v>
+      </c>
+      <c r="I6">
+        <v>18.8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>69</v>
+      </c>
+      <c r="K6" t="b">
+        <v>1</v>
+      </c>
+      <c r="L6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>67.140267005300004</v>
+      </c>
+      <c r="F7">
+        <v>-113.216152206</v>
+      </c>
+      <c r="H7">
+        <v>601.6</v>
+      </c>
+      <c r="I7">
+        <v>18.8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="b">
+        <v>1</v>
+      </c>
+      <c r="L7" t="b">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>67.140267005300004</v>
+      </c>
+      <c r="F8">
+        <v>-113.216152206</v>
+      </c>
+      <c r="H8">
+        <v>601.6</v>
+      </c>
+      <c r="I8">
+        <v>18.8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>69</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>0</v>
+      </c>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>67.138233</v>
+      </c>
+      <c r="F9">
+        <v>-113.214676</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="5">
+        <v>520.9</v>
+      </c>
+      <c r="I9" s="5">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J9" t="s">
+        <v>69</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10">
+        <v>67.138233</v>
+      </c>
+      <c r="F10">
+        <v>-113.214676</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10">
+        <v>520.9</v>
+      </c>
+      <c r="I10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>67.160099360199993</v>
+      </c>
+      <c r="F11">
+        <v>-112.794083372</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11">
+        <v>537</v>
+      </c>
+      <c r="I11">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" t="b">
+        <v>0</v>
+      </c>
+      <c r="N11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12">
+        <v>66.746940285999997</v>
+      </c>
+      <c r="F12">
+        <v>-112.744256083</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H12">
+        <v>616.29999999999995</v>
+      </c>
+      <c r="I12">
+        <v>28.2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12" t="b">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13">
+        <v>66.016999999999996</v>
+      </c>
+      <c r="F13">
+        <v>-111.529</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="6">
+        <v>173.1</v>
+      </c>
+      <c r="I13" s="5">
+        <v>1.3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13" t="b">
+        <v>0</v>
+      </c>
+      <c r="N13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14">
+        <v>70.715559999999996</v>
+      </c>
+      <c r="F14">
+        <v>-109.86109999999999</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14" t="b">
+        <v>0</v>
+      </c>
+      <c r="N14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15">
+        <v>73.290999999999997</v>
+      </c>
+      <c r="F15">
+        <v>-91.966999999999999</v>
+      </c>
+      <c r="G15" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H15" s="3">
+        <v>97.3</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.8</v>
+      </c>
+      <c r="J15" t="s">
+        <v>69</v>
+      </c>
+      <c r="K15" t="b">
+        <v>0</v>
+      </c>
+      <c r="L15" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16">
+        <v>73.334000000000003</v>
+      </c>
+      <c r="F16">
+        <v>-92.927000000000007</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.54</v>
+      </c>
+      <c r="H16" s="1">
+        <v>97.5</v>
+      </c>
+      <c r="I16" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K16" t="b">
+        <v>0</v>
+      </c>
+      <c r="L16" t="b">
+        <v>0</v>
+      </c>
+      <c r="N16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1">
+        <v>97.3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="J17" t="s">
+        <v>69</v>
+      </c>
+      <c r="K17" t="b">
+        <v>0</v>
+      </c>
+      <c r="L17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18">
+        <v>73.52</v>
+      </c>
+      <c r="F18">
+        <v>-90.956999999999994</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.61</v>
+      </c>
+      <c r="H18" s="1">
+        <v>96.4</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" t="b">
+        <v>0</v>
+      </c>
+      <c r="L18" t="b">
+        <v>0</v>
+      </c>
+      <c r="N18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <v>72.80444</v>
+      </c>
+      <c r="F19">
+        <v>-93.63306</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1">
+        <v>300</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1.2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>69</v>
+      </c>
+      <c r="K19" t="b">
+        <v>0</v>
+      </c>
+      <c r="L19" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20">
+        <v>73.117999999999995</v>
+      </c>
+      <c r="F20">
+        <v>-94.090999999999994</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="H20" s="1">
+        <v>98.2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>69</v>
+      </c>
+      <c r="K20" t="b">
+        <v>0</v>
+      </c>
+      <c r="L20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="E21">
+        <v>64.975999999999999</v>
+      </c>
+      <c r="F21">
+        <v>-111.01900000000001</v>
+      </c>
+      <c r="H21" s="5">
+        <v>321</v>
+      </c>
+      <c r="I21" s="5">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K21" t="b">
+        <v>0</v>
+      </c>
+      <c r="L21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="E22">
+        <v>64.658000000000001</v>
+      </c>
+      <c r="F22">
+        <v>-110.68</v>
+      </c>
+      <c r="H22" s="5">
+        <v>56.2</v>
+      </c>
+      <c r="I22" s="5">
+        <v>3.2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>69</v>
+      </c>
+      <c r="K22" t="b">
+        <v>0</v>
+      </c>
+      <c r="L22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23">
+        <v>64.715000000000003</v>
+      </c>
+      <c r="F23">
+        <v>-110.34699999999999</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="H23" s="5">
+        <v>45.4</v>
+      </c>
+      <c r="I23" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>94</v>
+      </c>
+      <c r="K23" t="b">
+        <v>0</v>
+      </c>
+      <c r="L23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24">
+        <v>64.411000000000001</v>
+      </c>
+      <c r="F24">
+        <v>-109.854</v>
+      </c>
+      <c r="H24" s="5">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="I24" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="J24" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" t="b">
+        <v>0</v>
+      </c>
+      <c r="L24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25">
+        <v>64.902000000000001</v>
+      </c>
+      <c r="F25">
+        <v>-110.908</v>
+      </c>
+      <c r="H25" s="5">
+        <v>61.1</v>
+      </c>
+      <c r="I25" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="J25" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" t="b">
+        <v>0</v>
+      </c>
+      <c r="L25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H26" s="5">
+        <v>613</v>
+      </c>
+      <c r="I26" s="5">
+        <v>6</v>
+      </c>
+      <c r="J26" t="s">
+        <v>90</v>
+      </c>
+      <c r="K26" t="b">
+        <v>0</v>
+      </c>
+      <c r="L26" t="b">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27">
+        <v>65.272999999999996</v>
+      </c>
+      <c r="F27">
+        <v>-111.51</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H27" s="5">
+        <v>52.1</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>90</v>
+      </c>
+      <c r="K27" t="b">
+        <v>0</v>
+      </c>
+      <c r="L27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E28">
+        <v>62.145000000000003</v>
+      </c>
+      <c r="F28">
+        <v>-113.825</v>
+      </c>
+      <c r="H28" s="5">
+        <v>441.4</v>
+      </c>
+      <c r="I28" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="J28" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29">
+        <v>64.3262</v>
+      </c>
+      <c r="F29">
+        <v>-109.81699999999999</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="5">
+        <v>69</v>
+      </c>
+      <c r="I29" s="5">
+        <v>6</v>
+      </c>
+      <c r="J29" t="s">
+        <v>69</v>
+      </c>
+      <c r="K29" t="b">
+        <v>0</v>
+      </c>
+      <c r="L29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="E30">
+        <v>63.435000000000002</v>
+      </c>
+      <c r="F30">
+        <v>-109.208</v>
+      </c>
+      <c r="H30" s="5">
+        <v>542.20000000000005</v>
+      </c>
+      <c r="I30" s="5">
+        <v>2.6</v>
+      </c>
+      <c r="J30" t="s">
+        <v>90</v>
+      </c>
+      <c r="K30" t="b">
+        <v>0</v>
+      </c>
+      <c r="L30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E31">
+        <v>63.593000000000004</v>
+      </c>
+      <c r="F31">
+        <v>-110.72799999999999</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="5">
+        <v>535</v>
+      </c>
+      <c r="I31" s="5">
+        <v>11</v>
+      </c>
+      <c r="J31" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" t="b">
+        <v>0</v>
+      </c>
+      <c r="L31" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commented code; cleaned up for LISA
</commit_message>
<xml_diff>
--- a/data/kimberlite_coords.xlsx
+++ b/data/kimberlite_coords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spencerzeigler/Documents/Flowers Lab/Arctic Kimberlite/canda-ahe-kimberlite-map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D7B71D-FB09-354D-8ECB-022AF91BBB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E367A03-4A9E-494B-8B22-951BEEAFE4F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="3460" windowWidth="21460" windowHeight="16520" xr2:uid="{271A1990-3C0E-BB45-A5DB-FD6F620B4979}"/>
+    <workbookView xWindow="920" yWindow="500" windowWidth="21460" windowHeight="16060" xr2:uid="{271A1990-3C0E-BB45-A5DB-FD6F620B4979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,7 +329,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -398,8 +398,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -718,7 +718,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1050,9 +1050,6 @@
       <c r="L8" t="b">
         <v>0</v>
       </c>
-      <c r="M8" t="b">
-        <v>0</v>
-      </c>
       <c r="N8" t="s">
         <v>37</v>
       </c>
@@ -1860,5 +1857,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>